<commit_message>
corrected data cleaning for pre/post/total fixation data
</commit_message>
<xml_diff>
--- a/analysis/participant_extractedmetrics/Participant110.xlsx
+++ b/analysis/participant_extractedmetrics/Participant110.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="99">
   <si>
     <t>total</t>
   </si>
@@ -96,187 +96,190 @@
     <t>Fixation duration (ms)</t>
   </si>
   <si>
-    <t>difference w/ new columns</t>
-  </si>
-  <si>
-    <t>post_condstate</t>
-  </si>
-  <si>
-    <t>post_excepton</t>
-  </si>
-  <si>
-    <t>post_loopstate</t>
-  </si>
-  <si>
-    <t>post_methocall2</t>
-  </si>
-  <si>
-    <t>post_methodec</t>
-  </si>
-  <si>
-    <t>post_operator</t>
-  </si>
-  <si>
-    <t>post_param</t>
-  </si>
-  <si>
-    <t>postexternalmethod</t>
-  </si>
-  <si>
-    <t>postliteral1</t>
-  </si>
-  <si>
-    <t>postliteral2</t>
-  </si>
-  <si>
-    <t>postsumaary</t>
-  </si>
-  <si>
-    <t>postvar1</t>
-  </si>
-  <si>
-    <t>psot_code</t>
-  </si>
-  <si>
-    <t>psot_methodcall</t>
-  </si>
-  <si>
-    <t>psot_var2</t>
+    <t>pre</t>
+  </si>
+  <si>
+    <t>conditional</t>
+  </si>
+  <si>
+    <t>statement</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>Fixation</t>
+  </si>
+  <si>
+    <t>based</t>
+  </si>
+  <si>
+    <t>metrics</t>
+  </si>
+  <si>
+    <t>Revisit</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Dwell</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>(ms)</t>
+  </si>
+  <si>
+    <t>(%)</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>fixation</t>
+  </si>
+  <si>
+    <t>arg 2</t>
+  </si>
+  <si>
+    <t>arg 3</t>
+  </si>
+  <si>
+    <t>arg 4</t>
+  </si>
+  <si>
+    <t>arg 5</t>
+  </si>
+  <si>
+    <t>arg 6</t>
+  </si>
+  <si>
+    <t>args 1</t>
+  </si>
+  <si>
+    <t>assing 1</t>
+  </si>
+  <si>
+    <t>assing 2</t>
+  </si>
+  <si>
+    <t>assing 3</t>
+  </si>
+  <si>
+    <t>cond body 1</t>
+  </si>
+  <si>
+    <t>cond body 2</t>
+  </si>
+  <si>
+    <t>cond body 3</t>
+  </si>
+  <si>
+    <t>conditionalstatement</t>
+  </si>
+  <si>
+    <t>conditionalstatment1</t>
+  </si>
+  <si>
+    <t>External call</t>
+  </si>
+  <si>
+    <t>External call 1</t>
+  </si>
+  <si>
+    <t>literal 1</t>
+  </si>
+  <si>
+    <t>literal 2</t>
+  </si>
+  <si>
+    <t>literal 3</t>
+  </si>
+  <si>
+    <t>literal 4</t>
+  </si>
+  <si>
+    <t>literal 5</t>
+  </si>
+  <si>
+    <t>loop body 3</t>
+  </si>
+  <si>
+    <t>loop body2</t>
+  </si>
+  <si>
+    <t>loop1</t>
+  </si>
+  <si>
+    <t>loop2</t>
+  </si>
+  <si>
+    <t>loop3</t>
+  </si>
+  <si>
+    <t>method call 1</t>
+  </si>
+  <si>
+    <t>method call 2</t>
+  </si>
+  <si>
+    <t>method call 3</t>
+  </si>
+  <si>
+    <t>method call 4</t>
+  </si>
+  <si>
+    <t>method call 5</t>
+  </si>
+  <si>
+    <t>method call 6</t>
+  </si>
+  <si>
+    <t>method call 7</t>
+  </si>
+  <si>
+    <t>method call 8</t>
+  </si>
+  <si>
+    <t>method call 9</t>
+  </si>
+  <si>
+    <t>methoddec</t>
+  </si>
+  <si>
+    <t>var name 1</t>
+  </si>
+  <si>
+    <t>var name 2</t>
+  </si>
+  <si>
+    <t>var name 3</t>
+  </si>
+  <si>
+    <t>var name 4</t>
+  </si>
+  <si>
+    <t>var name 5</t>
+  </si>
+  <si>
+    <t>var name 6</t>
+  </si>
+  <si>
+    <t>var name 7</t>
   </si>
   <si>
     <t>First fixation duration (ms)</t>
   </si>
   <si>
-    <t>arg 2</t>
-  </si>
-  <si>
-    <t>arg 3</t>
-  </si>
-  <si>
-    <t>arg 4</t>
-  </si>
-  <si>
-    <t>arg 5</t>
-  </si>
-  <si>
-    <t>arg 6</t>
-  </si>
-  <si>
-    <t>args 1</t>
-  </si>
-  <si>
-    <t>assing 1</t>
-  </si>
-  <si>
-    <t>assing 2</t>
-  </si>
-  <si>
-    <t>assing 3</t>
-  </si>
-  <si>
-    <t>cond body 1</t>
-  </si>
-  <si>
-    <t>cond body 2</t>
-  </si>
-  <si>
-    <t>cond body 3</t>
-  </si>
-  <si>
-    <t>conditionalstatement</t>
-  </si>
-  <si>
-    <t>conditionalstatment1</t>
-  </si>
-  <si>
-    <t>External call</t>
-  </si>
-  <si>
-    <t>External call 1</t>
-  </si>
-  <si>
-    <t>literal 1</t>
-  </si>
-  <si>
-    <t>literal 2</t>
-  </si>
-  <si>
-    <t>literal 3</t>
-  </si>
-  <si>
-    <t>literal 4</t>
-  </si>
-  <si>
-    <t>literal 5</t>
-  </si>
-  <si>
-    <t>loop body 3</t>
-  </si>
-  <si>
-    <t>loop body2</t>
-  </si>
-  <si>
-    <t>loop1</t>
-  </si>
-  <si>
-    <t>loop2</t>
-  </si>
-  <si>
-    <t>loop3</t>
-  </si>
-  <si>
-    <t>method call 1</t>
-  </si>
-  <si>
-    <t>method call 2</t>
-  </si>
-  <si>
-    <t>method call 3</t>
-  </si>
-  <si>
-    <t>method call 4</t>
-  </si>
-  <si>
-    <t>method call 5</t>
-  </si>
-  <si>
-    <t>method call 6</t>
-  </si>
-  <si>
-    <t>method call 7</t>
-  </si>
-  <si>
-    <t>method call 8</t>
-  </si>
-  <si>
-    <t>method call 9</t>
-  </si>
-  <si>
-    <t>methoddec</t>
-  </si>
-  <si>
-    <t>var name 1</t>
-  </si>
-  <si>
-    <t>var name 2</t>
-  </si>
-  <si>
-    <t>var name 3</t>
-  </si>
-  <si>
-    <t>var name 4</t>
-  </si>
-  <si>
-    <t>var name 5</t>
-  </si>
-  <si>
-    <t>var name 6</t>
-  </si>
-  <si>
-    <t>var name 7</t>
-  </si>
-  <si>
     <t>pre_gemini</t>
+  </si>
+  <si>
+    <t>post</t>
   </si>
   <si>
     <t>arg</t>
@@ -313,7 +316,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -324,6 +327,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -340,12 +348,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1004,863 +1021,755 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="3"/>
+      <c r="AO22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
+      <c r="AS22" s="3"/>
+      <c r="AT22" s="3"/>
+      <c r="AU22" s="3"/>
+      <c r="AV22" s="3"/>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="23">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="L23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="O23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="P23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="Q23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="R23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T13" s="1" t="s">
+      <c r="S23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
+      <c r="AO24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="C25" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R25" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="4">
+        <v>481.0</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="M26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" s="4">
+        <v>313.0</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="3"/>
+      <c r="AO26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+      <c r="AU26" s="3"/>
+      <c r="AV26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Z13" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AB13" s="1" t="s">
+      <c r="D27" s="4">
+        <v>8192.25</v>
+      </c>
+      <c r="E27" s="4">
+        <v>800.91</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="4">
+        <v>124078.4</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="4">
+        <v>200.26</v>
+      </c>
+      <c r="M27" s="4">
+        <v>1284.72</v>
+      </c>
+      <c r="N27" s="4">
+        <v>233.58</v>
+      </c>
+      <c r="O27" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="4">
+        <v>106930.4</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="4">
+        <v>200.26</v>
+      </c>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+      <c r="AT27" s="3"/>
+      <c r="AU27" s="3"/>
+      <c r="AV27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AC13" s="1" t="s">
+      <c r="D28" s="4">
+        <v>4.46</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="4">
+        <v>34.9</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="4">
+        <v>58.13</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="3"/>
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="3"/>
+      <c r="AU28" s="3"/>
+      <c r="AV28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AD13" s="1" t="s">
+      <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="4">
+        <v>341.34</v>
+      </c>
+      <c r="E29" s="4">
+        <v>400.45</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="4">
+        <v>257.96</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="4">
+        <v>200.26</v>
+      </c>
+      <c r="M29" s="4">
+        <v>428.24</v>
+      </c>
+      <c r="N29" s="4">
+        <v>233.58</v>
+      </c>
+      <c r="O29" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="4">
+        <v>341.63</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" s="4">
+        <v>200.26</v>
+      </c>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="3"/>
+      <c r="AO29" s="3"/>
+      <c r="AP29" s="3"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+      <c r="AT29" s="3"/>
+      <c r="AU29" s="3"/>
+      <c r="AV29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AE13" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AF13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI14" s="1"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="1">
-        <v>34.0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AA15" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF15" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="AG15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AI15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="1">
-        <v>481.0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>346.0</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC16" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF16" s="1">
-        <v>313.0</v>
-      </c>
-      <c r="AG16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="AI16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1">
-        <v>8192.25</v>
-      </c>
-      <c r="C17" s="1">
-        <v>800.91</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="1">
-        <v>124078.37</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="C30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="4">
+        <v>150.12</v>
+      </c>
+      <c r="F30" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="4">
+        <v>316.99</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="4">
         <v>200.26</v>
       </c>
-      <c r="K17" s="1">
-        <v>1284.72</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="N30" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="O30" s="4">
         <v>233.58</v>
       </c>
-      <c r="M17" s="1">
+      <c r="P30" s="4">
         <v>233.62</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R17" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X17" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="AA17" s="1">
-        <v>120549.36</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC17" s="1">
-        <v>834.24</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF17" s="1">
-        <v>106930.44</v>
-      </c>
-      <c r="AG17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH17" s="1">
+      <c r="Q30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T30" s="4">
+        <v>114.39</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V30" s="4">
         <v>200.26</v>
       </c>
-      <c r="AI17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1">
-        <v>4.46</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="1">
-        <v>34.9</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="M18" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R18" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X18" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z18" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="AA18" s="1">
-        <v>33.91</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC18" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="AD18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF18" s="1">
-        <v>58.13</v>
-      </c>
-      <c r="AG18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH18" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="AI18" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1">
-        <v>341.34</v>
-      </c>
-      <c r="C19" s="1">
-        <v>400.45</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="1">
-        <v>257.96</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="1">
-        <v>200.26</v>
-      </c>
-      <c r="K19" s="1">
-        <v>428.24</v>
-      </c>
-      <c r="L19" s="1">
-        <v>233.58</v>
-      </c>
-      <c r="M19" s="1">
-        <v>233.62</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R19" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X19" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="Y19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z19" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="AA19" s="1">
-        <v>348.41</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC19" s="1">
-        <v>417.12</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF19" s="1">
-        <v>341.63</v>
-      </c>
-      <c r="AG19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH19" s="1">
-        <v>200.26</v>
-      </c>
-      <c r="AI19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="1">
-        <v>150.12</v>
-      </c>
-      <c r="C20" s="1">
-        <v>233.62</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="1">
-        <v>316.99</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="1">
-        <v>200.26</v>
-      </c>
-      <c r="K20" s="1">
-        <v>233.62</v>
-      </c>
-      <c r="L20" s="1">
-        <v>233.58</v>
-      </c>
-      <c r="M20" s="1">
-        <v>233.62</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R20" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X20" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z20" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="AA20" s="1">
-        <v>250.31</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC20" s="1">
-        <v>467.17</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF20" s="1">
-        <v>114.39</v>
-      </c>
-      <c r="AG20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH20" s="1">
-        <v>200.26</v>
-      </c>
-      <c r="AI20" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="3"/>
+      <c r="AN30" s="3"/>
+      <c r="AO30" s="3"/>
+      <c r="AP30" s="3"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+      <c r="AT30" s="3"/>
+      <c r="AU30" s="3"/>
+      <c r="AV30" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1882,145 +1791,145 @@
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AP1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="AW1" s="1" t="s">
         <v>19</v>
@@ -2920,7 +2829,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -3072,145 +2981,145 @@
         <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="W13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="Z13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="AB13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AB13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AC13" s="1" t="s">
+      <c r="AD13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AD13" s="1" t="s">
+      <c r="AE13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AE13" s="1" t="s">
+      <c r="AF13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AG13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AG13" s="1" t="s">
+      <c r="AH13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AH13" s="1" t="s">
+      <c r="AI13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AI13" s="1" t="s">
+      <c r="AJ13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AJ13" s="1" t="s">
+      <c r="AK13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AK13" s="1" t="s">
+      <c r="AL13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AL13" s="1" t="s">
+      <c r="AM13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AM13" s="1" t="s">
+      <c r="AN13" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AN13" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="AO13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AP13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AQ13" s="1" t="s">
+      <c r="AR13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AR13" s="1" t="s">
+      <c r="AS13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AS13" s="1" t="s">
+      <c r="AT13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AT13" s="1" t="s">
+      <c r="AU13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AU13" s="1" t="s">
+      <c r="AV13" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AV13" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="AW13" s="1" t="s">
         <v>19</v>
@@ -4110,7 +4019,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>22</v>
@@ -4257,7 +4166,1133 @@
         <v>19</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV24" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="M26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="P26" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Y26" s="4">
+        <v>28.0</v>
+      </c>
+      <c r="Z26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AA26" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AH26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AI26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AJ26" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AK26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AM26" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="AN26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO26" s="4">
+        <v>47.0</v>
+      </c>
+      <c r="AP26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K27" s="4">
+        <v>74.0</v>
+      </c>
+      <c r="L27" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="M27" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="N27" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="O27" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="P27" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="4">
+        <v>301.0</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X27" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>60.0</v>
+      </c>
+      <c r="Z27" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="AA27" s="4">
+        <v>48.0</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AH27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="AI27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="AJ27" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AK27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL27" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="AM27" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="AN27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO27" s="4">
+        <v>219.0</v>
+      </c>
+      <c r="AP27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1185.03</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3073.27</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="K28" s="4">
+        <v>27389.6</v>
+      </c>
+      <c r="L28" s="4">
+        <v>5389.45</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1065.01</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1698.0</v>
+      </c>
+      <c r="O28" s="4">
+        <v>448.36</v>
+      </c>
+      <c r="P28" s="4">
+        <v>3558.03</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="4">
+        <v>72517.25</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X28" s="4">
+        <v>240.29</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>23851.09</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>3155.16</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>15184.96</v>
+      </c>
+      <c r="AB28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD28" s="4">
+        <v>1185.03</v>
+      </c>
+      <c r="AE28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG28" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="AH28" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="AI28" s="4">
+        <v>2722.74</v>
+      </c>
+      <c r="AJ28" s="4">
+        <v>1820.23</v>
+      </c>
+      <c r="AK28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL28" s="4">
+        <v>544.64</v>
+      </c>
+      <c r="AM28" s="4">
+        <v>1698.0</v>
+      </c>
+      <c r="AN28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO28" s="4">
+        <v>76740.81</v>
+      </c>
+      <c r="AP28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1.14</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="K29" s="4">
+        <v>10.16</v>
+      </c>
+      <c r="L29" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="P29" s="4">
+        <v>1.32</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="4">
+        <v>26.9</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X29" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="Y29" s="4">
+        <v>8.85</v>
+      </c>
+      <c r="Z29" s="4">
+        <v>1.17</v>
+      </c>
+      <c r="AA29" s="4">
+        <v>5.63</v>
+      </c>
+      <c r="AB29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD29" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="AE29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG29" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="AH29" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="AI29" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="AJ29" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="AK29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL29" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AM29" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="AN29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO29" s="4">
+        <v>28.47</v>
+      </c>
+      <c r="AP29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV29" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1185.03</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="4">
+        <v>512.21</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="K30" s="4">
+        <v>370.13</v>
+      </c>
+      <c r="L30" s="4">
+        <v>359.3</v>
+      </c>
+      <c r="M30" s="4">
+        <v>532.51</v>
+      </c>
+      <c r="N30" s="4">
+        <v>424.5</v>
+      </c>
+      <c r="O30" s="4">
+        <v>224.18</v>
+      </c>
+      <c r="P30" s="4">
+        <v>355.8</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" s="4">
+        <v>240.92</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X30" s="4">
+        <v>120.15</v>
+      </c>
+      <c r="Y30" s="4">
+        <v>397.52</v>
+      </c>
+      <c r="Z30" s="4">
+        <v>450.74</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>316.35</v>
+      </c>
+      <c r="AB30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD30" s="4">
+        <v>1185.03</v>
+      </c>
+      <c r="AE30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG30" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="AH30" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="AI30" s="4">
+        <v>453.79</v>
+      </c>
+      <c r="AJ30" s="4">
+        <v>455.06</v>
+      </c>
+      <c r="AK30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL30" s="4">
+        <v>272.32</v>
+      </c>
+      <c r="AM30" s="4">
+        <v>424.5</v>
+      </c>
+      <c r="AN30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO30" s="4">
+        <v>350.41</v>
+      </c>
+      <c r="AP30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1185.03</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="4">
+        <v>350.36</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="K31" s="4">
+        <v>350.36</v>
+      </c>
+      <c r="L31" s="4">
+        <v>192.24</v>
+      </c>
+      <c r="M31" s="4">
+        <v>712.7</v>
+      </c>
+      <c r="N31" s="4">
+        <v>176.4</v>
+      </c>
+      <c r="O31" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="P31" s="4">
+        <v>266.57</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S31" s="4">
+        <v>233.56</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X31" s="4">
+        <v>80.13</v>
+      </c>
+      <c r="Y31" s="4">
+        <v>350.36</v>
+      </c>
+      <c r="Z31" s="4">
+        <v>192.24</v>
+      </c>
+      <c r="AA31" s="4">
+        <v>166.88</v>
+      </c>
+      <c r="AB31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD31" s="4">
+        <v>1185.03</v>
+      </c>
+      <c r="AE31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG31" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="AH31" s="4">
+        <v>336.27</v>
+      </c>
+      <c r="AI31" s="4">
+        <v>192.24</v>
+      </c>
+      <c r="AJ31" s="4">
+        <v>266.57</v>
+      </c>
+      <c r="AK31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL31" s="4">
+        <v>160.22</v>
+      </c>
+      <c r="AM31" s="4">
+        <v>176.4</v>
+      </c>
+      <c r="AN31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO31" s="4">
+        <v>350.36</v>
+      </c>
+      <c r="AP31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV31" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A25:B25"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4277,43 +5312,43 @@
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
@@ -4322,19 +5357,19 @@
         <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>15</v>
@@ -4343,14 +5378,36 @@
         <v>16</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -4429,6 +5486,28 @@
         <v>19</v>
       </c>
       <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -4509,6 +5588,28 @@
       <c r="Z3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -4589,6 +5690,28 @@
       <c r="Z4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -4669,6 +5792,28 @@
       <c r="Z5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -4749,6 +5894,28 @@
       <c r="Z6" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -4829,10 +5996,32 @@
       <c r="Z7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -4909,49 +6098,71 @@
       <c r="Z8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>6</v>
@@ -4960,19 +6171,19 @@
         <v>10</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="U12" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>15</v>
@@ -4981,14 +6192,36 @@
         <v>16</v>
       </c>
       <c r="X12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Y12" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="Z12" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -5067,6 +6300,28 @@
         <v>19</v>
       </c>
       <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -5147,6 +6402,28 @@
       <c r="Z14" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -5227,6 +6504,28 @@
       <c r="Z15" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -5307,6 +6606,28 @@
       <c r="Z16" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -5387,6 +6708,28 @@
       <c r="Z17" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -5467,10 +6810,32 @@
       <c r="Z18" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
@@ -5547,8 +6912,834 @@
       <c r="Z19" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="3"/>
+      <c r="AO22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
+      <c r="AS22" s="3"/>
+      <c r="AT22" s="3"/>
+      <c r="AU22" s="3"/>
+      <c r="AV22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
+      <c r="AO24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="O25" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="P25" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="S25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="T25" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W25" s="4">
+        <v>28.0</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>290.0</v>
+      </c>
+      <c r="P26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="S26" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="T26" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" s="4">
+        <v>188.0</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="3"/>
+      <c r="AO26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+      <c r="AU26" s="3"/>
+      <c r="AV26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="4">
+        <v>3295.06</v>
+      </c>
+      <c r="G27" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="H27" s="4">
+        <v>867.57</v>
+      </c>
+      <c r="I27" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="J27" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="K27" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="4">
+        <v>333.68</v>
+      </c>
+      <c r="O27" s="4">
+        <v>74404.08</v>
+      </c>
+      <c r="P27" s="4">
+        <v>1334.75</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="S27" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="T27" s="4">
+        <v>867.57</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" s="4">
+        <v>60673.49</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+      <c r="AT27" s="3"/>
+      <c r="AU27" s="3"/>
+      <c r="AV27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1.56</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="O28" s="4">
+        <v>35.27</v>
+      </c>
+      <c r="P28" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="S28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="T28" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W28" s="4">
+        <v>28.72</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="3"/>
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="3"/>
+      <c r="AU28" s="3"/>
+      <c r="AV28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="4">
+        <v>329.51</v>
+      </c>
+      <c r="G29" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="H29" s="4">
+        <v>433.78</v>
+      </c>
+      <c r="I29" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="J29" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="K29" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="4">
+        <v>333.68</v>
+      </c>
+      <c r="O29" s="4">
+        <v>256.57</v>
+      </c>
+      <c r="P29" s="4">
+        <v>333.69</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="S29" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="T29" s="4">
+        <v>433.78</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W29" s="4">
+        <v>322.73</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="3"/>
+      <c r="AO29" s="3"/>
+      <c r="AP29" s="3"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+      <c r="AT29" s="3"/>
+      <c r="AU29" s="3"/>
+      <c r="AV29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="4">
+        <v>175.19</v>
+      </c>
+      <c r="G30" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="H30" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="I30" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="J30" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="K30" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="4">
+        <v>333.68</v>
+      </c>
+      <c r="O30" s="4">
+        <v>216.87</v>
+      </c>
+      <c r="P30" s="4">
+        <v>233.56</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R30" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="S30" s="4">
+        <v>233.62</v>
+      </c>
+      <c r="T30" s="4">
+        <v>533.89</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W30" s="4">
+        <v>317.0</v>
+      </c>
+      <c r="X30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="3"/>
+      <c r="AN30" s="3"/>
+      <c r="AO30" s="3"/>
+      <c r="AP30" s="3"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+      <c r="AT30" s="3"/>
+      <c r="AU30" s="3"/>
+      <c r="AV30" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="A24:B24"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>